<commit_message>
more final animation final stuff. final.
</commit_message>
<xml_diff>
--- a/animations/fragment-skid-and-reverse-b.xlsx
+++ b/animations/fragment-skid-and-reverse-b.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B1C31A-0152-42FC-A3F5-B51AD8345881}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0BD090-8B09-DC4D-BD09-0AE837892452}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="465" windowWidth="49215" windowHeight="28335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="50280" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,18 +428,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
-      <selection activeCell="AS24" sqref="AS24:BA40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
+      <selection activeCell="AY37" sqref="AY37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="20" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="66" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="20" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="66" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -643,7 +639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -672,7 +668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -704,7 +700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>1</v>
       </c>
@@ -736,7 +732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
       <c r="F5">
         <v>1</v>
       </c>
@@ -768,7 +764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="H6">
         <v>1</v>
       </c>
@@ -806,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
       <c r="I7">
         <v>1</v>
       </c>
@@ -856,7 +852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
       <c r="J8">
         <v>1</v>
       </c>
@@ -921,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
       <c r="O9">
         <v>1</v>
       </c>
@@ -992,7 +988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
       <c r="T10">
         <v>1</v>
       </c>
@@ -1063,7 +1059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
       <c r="AA11">
         <v>1</v>
       </c>
@@ -1122,7 +1118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
       <c r="AH12">
         <v>1</v>
       </c>
@@ -1166,7 +1162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
       <c r="AL13">
         <v>1</v>
       </c>
@@ -1201,7 +1197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
       <c r="AO14">
         <v>1</v>
       </c>
@@ -1233,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
       <c r="AO15" s="2"/>
       <c r="AP15" s="3"/>
       <c r="AS15">
@@ -1261,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
       <c r="AO16" s="2"/>
       <c r="AP16" s="3"/>
       <c r="AT16">
@@ -1289,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="17" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AO17" s="2"/>
       <c r="AP17" s="3"/>
       <c r="AU17" s="2">
@@ -1323,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="18" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AO18" s="3"/>
       <c r="AP18" s="2"/>
       <c r="AU18" s="3"/>
@@ -1361,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="19" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AO19" s="3"/>
       <c r="AP19" s="2"/>
       <c r="AU19" s="3"/>
@@ -1393,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="20" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AO20" s="3"/>
       <c r="AP20" s="2"/>
       <c r="AU20">
@@ -1421,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="21" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AO21" s="3"/>
       <c r="AP21" s="2"/>
       <c r="AR21">
@@ -1458,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="22" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AO22" s="3"/>
       <c r="AP22" s="2"/>
       <c r="AR22">
@@ -1486,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="23" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AP23" s="2"/>
       <c r="AS23">
         <v>1</v>
@@ -1507,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="24" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AP24" s="2"/>
       <c r="AT24">
         <v>1</v>
@@ -1531,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="25" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AP25" s="2"/>
       <c r="AS25">
         <v>1</v>
@@ -1552,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="26" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AP26" s="2"/>
       <c r="AS26">
         <v>1</v>
@@ -1573,7 +1569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="27" spans="41:58" x14ac:dyDescent="0.2">
       <c r="AP27" s="2"/>
       <c r="AS27">
         <v>1</v>
@@ -1594,108 +1590,264 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="41:58" x14ac:dyDescent="0.25">
+    <row r="28" spans="41:58" x14ac:dyDescent="0.2">
+      <c r="AS28">
+        <v>1</v>
+      </c>
+      <c r="AT28">
+        <v>3</v>
+      </c>
       <c r="AU28">
         <v>8</v>
       </c>
       <c r="AV28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="41:58" x14ac:dyDescent="0.25">
+      <c r="AW28">
+        <v>3</v>
+      </c>
+      <c r="AX28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="41:58" x14ac:dyDescent="0.2">
+      <c r="AS29">
+        <v>1</v>
+      </c>
+      <c r="AT29">
+        <v>3</v>
+      </c>
       <c r="AU29">
         <v>8</v>
       </c>
       <c r="AV29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="41:58" x14ac:dyDescent="0.25">
+      <c r="AW29">
+        <v>3</v>
+      </c>
+      <c r="AX29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="41:58" x14ac:dyDescent="0.2">
+      <c r="AS30">
+        <v>1</v>
+      </c>
+      <c r="AT30">
+        <v>3</v>
+      </c>
       <c r="AU30">
         <v>8</v>
       </c>
       <c r="AV30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="41:58" x14ac:dyDescent="0.25">
+      <c r="AW30">
+        <v>3</v>
+      </c>
+      <c r="AX30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="41:58" x14ac:dyDescent="0.2">
+      <c r="AS31">
+        <v>1</v>
+      </c>
+      <c r="AT31">
+        <v>3</v>
+      </c>
       <c r="AU31">
         <v>8</v>
       </c>
       <c r="AV31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="41:58" x14ac:dyDescent="0.25">
+      <c r="AW31">
+        <v>3</v>
+      </c>
+      <c r="AX31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="41:58" x14ac:dyDescent="0.2">
+      <c r="AS32">
+        <v>1</v>
+      </c>
+      <c r="AT32">
+        <v>3</v>
+      </c>
       <c r="AU32">
         <v>8</v>
       </c>
       <c r="AV32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW32">
+        <v>3</v>
+      </c>
+      <c r="AX32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS33">
+        <v>1</v>
+      </c>
+      <c r="AT33">
+        <v>3</v>
+      </c>
       <c r="AU33">
         <v>8</v>
       </c>
       <c r="AV33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW33">
+        <v>3</v>
+      </c>
+      <c r="AX33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS34">
+        <v>1</v>
+      </c>
+      <c r="AT34">
+        <v>3</v>
+      </c>
       <c r="AU34">
         <v>8</v>
       </c>
       <c r="AV34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW34">
+        <v>3</v>
+      </c>
+      <c r="AX34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS35">
+        <v>1</v>
+      </c>
+      <c r="AT35">
+        <v>3</v>
+      </c>
       <c r="AU35">
         <v>8</v>
       </c>
       <c r="AV35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW35">
+        <v>3</v>
+      </c>
+      <c r="AX35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS36">
+        <v>1</v>
+      </c>
+      <c r="AT36">
+        <v>3</v>
+      </c>
       <c r="AU36">
         <v>8</v>
       </c>
       <c r="AV36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW36">
+        <v>3</v>
+      </c>
+      <c r="AX36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS37">
+        <v>1</v>
+      </c>
+      <c r="AT37">
+        <v>3</v>
+      </c>
       <c r="AU37">
         <v>8</v>
       </c>
       <c r="AV37">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW37">
+        <v>3</v>
+      </c>
+      <c r="AX37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS38">
+        <v>1</v>
+      </c>
+      <c r="AT38">
+        <v>3</v>
+      </c>
       <c r="AU38">
         <v>8</v>
       </c>
       <c r="AV38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW38">
+        <v>3</v>
+      </c>
+      <c r="AX38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS39">
+        <v>1</v>
+      </c>
+      <c r="AT39">
+        <v>3</v>
+      </c>
       <c r="AU39">
         <v>8</v>
       </c>
       <c r="AV39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="47:48" x14ac:dyDescent="0.25">
+      <c r="AW39">
+        <v>3</v>
+      </c>
+      <c r="AX39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="45:50" x14ac:dyDescent="0.2">
+      <c r="AS40">
+        <v>1</v>
+      </c>
+      <c r="AT40">
+        <v>3</v>
+      </c>
       <c r="AU40">
         <v>8</v>
       </c>
       <c r="AV40">
         <v>8</v>
+      </c>
+      <c r="AW40">
+        <v>3</v>
+      </c>
+      <c r="AX40">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>